<commit_message>
updated tab file name
</commit_message>
<xml_diff>
--- a/TableS1.xlsx
+++ b/TableS1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="154">
   <si>
     <t>Figure</t>
   </si>
@@ -53,7 +53,7 @@
     <t>Htz1</t>
   </si>
   <si>
-    <t>Mock</t>
+    <t>0min</t>
   </si>
   <si>
     <t>XO</t>
@@ -251,90 +251,87 @@
     <t>15941sacCer3.tab</t>
   </si>
   <si>
+    <t>6min</t>
+  </si>
+  <si>
+    <t>50503sacCer3.tab</t>
+  </si>
+  <si>
+    <t>9min</t>
+  </si>
+  <si>
+    <t>50504sacCer3.tab</t>
+  </si>
+  <si>
+    <t>12min</t>
+  </si>
+  <si>
+    <t>50505sacCer3.tab</t>
+  </si>
+  <si>
+    <t>15min</t>
+  </si>
+  <si>
+    <t>50506sacCer3.tab</t>
+  </si>
+  <si>
+    <t>50422sacCer3.tab;51835sacCer3.tab</t>
+  </si>
+  <si>
+    <t>51825sacCer3.tab;51827sacCer3.tab</t>
+  </si>
+  <si>
+    <t>53826sacCer3.tab</t>
+  </si>
+  <si>
+    <t>53409sacCer3.tab</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>56422sacCer3.tab;56428sacCer3.tab</t>
+  </si>
+  <si>
+    <t>56423sacCer3.tab;56429sacCer3.tab</t>
+  </si>
+  <si>
+    <t>56424sacCer3.tab;56430sacCer3.tab</t>
+  </si>
+  <si>
+    <t>51829sacCer3.tab</t>
+  </si>
+  <si>
+    <t>51830sacCer3.tab</t>
+  </si>
+  <si>
+    <t>51831sacCer3.tab</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>19325sacCer3.tab;19339sacCer3.tab;50519sacCer3.tab</t>
+  </si>
+  <si>
+    <t>32321sacCer3.tab;50520sacCer3.tab</t>
+  </si>
+  <si>
+    <t>32322sacCer3.tab;50521sacCer3.tab</t>
+  </si>
+  <si>
+    <t>32323sacCer3.tab;50522sacCer3.tab</t>
+  </si>
+  <si>
+    <t>32324sacCer3.tab;50523sacCer3.tab</t>
+  </si>
+  <si>
+    <t>32325sacCer3.tab;50524sacCer3.tab</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
-    <t>6min</t>
-  </si>
-  <si>
-    <t>50503sacCer3.tab</t>
-  </si>
-  <si>
-    <t>9min</t>
-  </si>
-  <si>
-    <t>50504sacCer3.tab</t>
-  </si>
-  <si>
-    <t>12min</t>
-  </si>
-  <si>
-    <t>50505sacCer3.tab</t>
-  </si>
-  <si>
-    <t>15min</t>
-  </si>
-  <si>
-    <t>50506sacCer3.tab</t>
-  </si>
-  <si>
-    <t>50422sacCer3.tab;51835sacCer3.tab</t>
-  </si>
-  <si>
-    <t>51825sacCer3.tab;51827sacCer3.tab</t>
-  </si>
-  <si>
-    <t>53826sacCer3.tab</t>
-  </si>
-  <si>
-    <t>53409sacCer3.tab</t>
-  </si>
-  <si>
-    <t>0min</t>
-  </si>
-  <si>
-    <t>PS</t>
-  </si>
-  <si>
-    <t>56422sacCer3.tab;56428sacCer3.tab</t>
-  </si>
-  <si>
-    <t>56423sacCer3.tab;56429sacCer3.tab</t>
-  </si>
-  <si>
-    <t>56424sacCer3.tab;56430sacCer3.tab</t>
-  </si>
-  <si>
-    <t>51829sacCer3.tab</t>
-  </si>
-  <si>
-    <t>51830sacCer3.tab</t>
-  </si>
-  <si>
-    <t>51831sacCer3.tab</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>19325sacCer3.tab;19339sacCer3.tab;50519sacCer3.tab</t>
-  </si>
-  <si>
-    <t>32321sacCer3.tab;50520sacCer3.tab</t>
-  </si>
-  <si>
-    <t>32322sacCer3.tab;50521sacCer3.tab</t>
-  </si>
-  <si>
-    <t>32323sacCer3.tab;50522sacCer3.tab</t>
-  </si>
-  <si>
-    <t>32324sacCer3.tab;50523sacCer3.tab</t>
-  </si>
-  <si>
-    <t>32325sacCer3.tab;50524sacCer3.tab</t>
-  </si>
-  <si>
     <t>S2</t>
   </si>
   <si>
@@ -405,6 +402,84 @@
   </si>
   <si>
     <t>See</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>Sgf11</t>
+  </si>
+  <si>
+    <t>13365sacCer3.tab</t>
+  </si>
+  <si>
+    <t>Ubp8</t>
+  </si>
+  <si>
+    <t>11962sacCer3.tab</t>
+  </si>
+  <si>
+    <t>Spt7</t>
+  </si>
+  <si>
+    <t>15907sacCer3.tab</t>
+  </si>
+  <si>
+    <t>13366sacCer3.tab</t>
+  </si>
+  <si>
+    <t>11963sacCer3.tab</t>
+  </si>
+  <si>
+    <t>15908sacCer3.tab</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>Rsc1</t>
+  </si>
+  <si>
+    <t>15809sacCer3.tab</t>
+  </si>
+  <si>
+    <t>Rsc3</t>
+  </si>
+  <si>
+    <t>11848sacCer3.tab</t>
+  </si>
+  <si>
+    <t>Rsc58</t>
+  </si>
+  <si>
+    <t>11855sacCer3.tab</t>
+  </si>
+  <si>
+    <t>Rsc6</t>
+  </si>
+  <si>
+    <t>11856sacCer3.tab</t>
+  </si>
+  <si>
+    <t>Sth1</t>
+  </si>
+  <si>
+    <t>15805sacCer3.tab</t>
+  </si>
+  <si>
+    <t>15165sacCer3.tab</t>
+  </si>
+  <si>
+    <t>15815sacCer3.tab</t>
+  </si>
+  <si>
+    <t>15810sacCer3.tab</t>
+  </si>
+  <si>
+    <t>15814sacCer3.tab</t>
+  </si>
+  <si>
+    <t>15812sacCer3.tab</t>
   </si>
   <si>
     <t>S8</t>
@@ -699,22 +774,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:172"/>
+  <dimension ref="1:193"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G160" activeCellId="0" sqref="G160"/>
+      <selection pane="bottomLeft" activeCell="G170" activeCellId="0" sqref="G170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="3" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="154.567441860465"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="3" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="159.367441860465"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2394,28 +2469,41 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E75" s="9"/>
-      <c r="F75" s="9"/>
-    </row>
-    <row r="76" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="10"/>
-      <c r="B76" s="11"/>
-      <c r="E76" s="13"/>
-      <c r="F76" s="13"/>
-      <c r="AMD76" s="0"/>
-      <c r="AME76" s="0"/>
-      <c r="AMF76" s="0"/>
-      <c r="AMG76" s="0"/>
-      <c r="AMH76" s="0"/>
-      <c r="AMI76" s="0"/>
-      <c r="AMJ76" s="0"/>
+    <row r="75" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="10"/>
+      <c r="B75" s="11"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="AMD75" s="0"/>
+      <c r="AME75" s="0"/>
+      <c r="AMF75" s="0"/>
+      <c r="AMG75" s="0"/>
+      <c r="AMH75" s="0"/>
+      <c r="AMI75" s="0"/>
+      <c r="AMJ75" s="0"/>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G76" s="0" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
@@ -2431,13 +2519,13 @@
         <v>55</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F77" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2445,7 +2533,7 @@
         <v>5</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="C78" s="0" t="s">
         <v>54</v>
@@ -2454,13 +2542,13 @@
         <v>55</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F78" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2477,13 +2565,13 @@
         <v>55</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F79" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2500,13 +2588,13 @@
         <v>55</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="F80" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2523,13 +2611,13 @@
         <v>55</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F81" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2546,13 +2634,13 @@
         <v>55</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F82" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2569,50 +2657,50 @@
         <v>55</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F83" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="E84" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F84" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G84" s="0" t="s">
+    </row>
+    <row r="84" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="10"/>
+      <c r="B84" s="11"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+      <c r="AMD84" s="0"/>
+      <c r="AME84" s="0"/>
+      <c r="AMF84" s="0"/>
+      <c r="AMG84" s="0"/>
+      <c r="AMH84" s="0"/>
+      <c r="AMI84" s="0"/>
+      <c r="AMJ84" s="0"/>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G85" s="0" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="85" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="10"/>
-      <c r="B85" s="11"/>
-      <c r="E85" s="13"/>
-      <c r="F85" s="13"/>
-      <c r="AMD85" s="0"/>
-      <c r="AME85" s="0"/>
-      <c r="AMF85" s="0"/>
-      <c r="AMG85" s="0"/>
-      <c r="AMH85" s="0"/>
-      <c r="AMI85" s="0"/>
-      <c r="AMJ85" s="0"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="n">
@@ -2622,10 +2710,10 @@
         <v>50</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E86" s="9" t="s">
         <v>10</v>
@@ -2642,13 +2730,13 @@
         <v>6</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E87" s="9" t="s">
         <v>10</v>
@@ -2657,7 +2745,7 @@
         <v>11</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2674,13 +2762,13 @@
         <v>35</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F88" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2697,13 +2785,13 @@
         <v>35</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="F89" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2714,19 +2802,19 @@
         <v>68</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="F90" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2743,13 +2831,13 @@
         <v>31</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F91" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2766,50 +2854,50 @@
         <v>31</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="F92" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C93" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D93" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="F93" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G93" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="10"/>
+      <c r="B93" s="11"/>
+      <c r="E93" s="13"/>
+      <c r="F93" s="13"/>
+      <c r="AMD93" s="0"/>
+      <c r="AME93" s="0"/>
+      <c r="AMF93" s="0"/>
+      <c r="AMG93" s="0"/>
+      <c r="AMH93" s="0"/>
+      <c r="AMI93" s="0"/>
+      <c r="AMJ93" s="0"/>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F94" s="9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="94" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="10"/>
-      <c r="B94" s="11"/>
-      <c r="E94" s="13"/>
-      <c r="F94" s="13"/>
-      <c r="AMD94" s="0"/>
-      <c r="AME94" s="0"/>
-      <c r="AMF94" s="0"/>
-      <c r="AMG94" s="0"/>
-      <c r="AMH94" s="0"/>
-      <c r="AMI94" s="0"/>
-      <c r="AMJ94" s="0"/>
+      <c r="G94" s="0" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="n">
@@ -2825,13 +2913,13 @@
         <v>23</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="F95" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G95" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="G95" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2848,13 +2936,13 @@
         <v>23</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="F96" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2862,7 +2950,7 @@
         <v>7</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="C97" s="0" t="s">
         <v>22</v>
@@ -2871,13 +2959,13 @@
         <v>23</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="F97" s="9" t="s">
-        <v>90</v>
+        <v>11</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2894,13 +2982,13 @@
         <v>23</v>
       </c>
       <c r="E98" s="9" t="s">
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="F98" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G98" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2917,13 +3005,13 @@
         <v>23</v>
       </c>
       <c r="E99" s="9" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="F99" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2940,13 +3028,13 @@
         <v>23</v>
       </c>
       <c r="E100" s="9" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="F100" s="9" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2963,13 +3051,13 @@
         <v>23</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="F101" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G101" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="G101" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2986,54 +3074,54 @@
         <v>23</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="F102" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G102" s="0" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C103" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D103" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E103" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="F103" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="G103" s="0" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="104" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="15"/>
-      <c r="B104" s="16"/>
-      <c r="E104" s="18"/>
-      <c r="F104" s="18"/>
-      <c r="AMD104" s="0"/>
-      <c r="AME104" s="0"/>
-      <c r="AMF104" s="0"/>
-      <c r="AMG104" s="0"/>
-      <c r="AMH104" s="0"/>
-      <c r="AMI104" s="0"/>
-      <c r="AMJ104" s="0"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="103" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="15"/>
+      <c r="B103" s="16"/>
+      <c r="E103" s="18"/>
+      <c r="F103" s="18"/>
+      <c r="AMD103" s="0"/>
+      <c r="AME103" s="0"/>
+      <c r="AMF103" s="0"/>
+      <c r="AMG103" s="0"/>
+      <c r="AMH103" s="0"/>
+      <c r="AMI103" s="0"/>
+      <c r="AMJ103" s="0"/>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D104" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F104" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G104" s="0" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>50</v>
@@ -3045,18 +3133,18 @@
         <v>27</v>
       </c>
       <c r="E105" s="9" t="s">
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="F105" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G105" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>50</v>
@@ -3068,18 +3156,18 @@
         <v>27</v>
       </c>
       <c r="E106" s="9" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="F106" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G106" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>50</v>
@@ -3091,18 +3179,18 @@
         <v>27</v>
       </c>
       <c r="E107" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F107" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G107" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>50</v>
@@ -3114,18 +3202,18 @@
         <v>27</v>
       </c>
       <c r="E108" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F108" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G108" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>50</v>
@@ -3137,105 +3225,105 @@
         <v>27</v>
       </c>
       <c r="E109" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F109" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G109" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E110" s="9" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="F110" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G110" s="0" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E111" s="9" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="F111" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G111" s="0" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E112" s="9" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="F112" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G112" s="0" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E113" s="9" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="F113" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G113" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="114" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3253,7 +3341,7 @@
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>7</v>
@@ -3265,7 +3353,7 @@
         <v>27</v>
       </c>
       <c r="E115" s="9" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="F115" s="9" t="s">
         <v>11</v>
@@ -3276,7 +3364,7 @@
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>7</v>
@@ -3299,7 +3387,7 @@
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>7</v>
@@ -3311,18 +3399,18 @@
         <v>27</v>
       </c>
       <c r="E117" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F117" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G117" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>7</v>
@@ -3334,18 +3422,18 @@
         <v>27</v>
       </c>
       <c r="E118" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F118" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G118" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>7</v>
@@ -3357,18 +3445,18 @@
         <v>27</v>
       </c>
       <c r="E119" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F119" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G119" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>7</v>
@@ -3380,18 +3468,18 @@
         <v>27</v>
       </c>
       <c r="E120" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F120" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G120" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>7</v>
@@ -3403,7 +3491,7 @@
         <v>16</v>
       </c>
       <c r="E121" s="9" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="F121" s="9" t="s">
         <v>11</v>
@@ -3414,7 +3502,7 @@
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>7</v>
@@ -3437,7 +3525,7 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>7</v>
@@ -3449,18 +3537,18 @@
         <v>16</v>
       </c>
       <c r="E123" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F123" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G123" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>7</v>
@@ -3472,18 +3560,18 @@
         <v>16</v>
       </c>
       <c r="E124" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F124" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G124" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>7</v>
@@ -3495,18 +3583,18 @@
         <v>16</v>
       </c>
       <c r="E125" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F125" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G125" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>7</v>
@@ -3518,13 +3606,13 @@
         <v>16</v>
       </c>
       <c r="E126" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F126" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G126" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="127" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3542,7 +3630,7 @@
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>50</v>
@@ -3554,7 +3642,7 @@
         <v>16</v>
       </c>
       <c r="E128" s="9" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="F128" s="9" t="s">
         <v>11</v>
@@ -3565,7 +3653,7 @@
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>50</v>
@@ -3588,7 +3676,7 @@
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>50</v>
@@ -3600,18 +3688,18 @@
         <v>16</v>
       </c>
       <c r="E130" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F130" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G130" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>50</v>
@@ -3623,18 +3711,18 @@
         <v>16</v>
       </c>
       <c r="E131" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F131" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G131" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>50</v>
@@ -3646,18 +3734,18 @@
         <v>16</v>
       </c>
       <c r="E132" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F132" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G132" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>50</v>
@@ -3669,18 +3757,18 @@
         <v>16</v>
       </c>
       <c r="E133" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F133" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G133" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>50</v>
@@ -3692,7 +3780,7 @@
         <v>58</v>
       </c>
       <c r="E134" s="9" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="F134" s="9" t="s">
         <v>11</v>
@@ -3703,7 +3791,7 @@
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>50</v>
@@ -3726,7 +3814,7 @@
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>50</v>
@@ -3738,18 +3826,18 @@
         <v>58</v>
       </c>
       <c r="E136" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F136" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G136" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>50</v>
@@ -3761,7 +3849,7 @@
         <v>23</v>
       </c>
       <c r="E137" s="9" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="F137" s="9" t="s">
         <v>11</v>
@@ -3772,7 +3860,7 @@
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>50</v>
@@ -3795,7 +3883,7 @@
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>50</v>
@@ -3807,18 +3895,18 @@
         <v>23</v>
       </c>
       <c r="E139" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F139" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G139" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>50</v>
@@ -3830,7 +3918,7 @@
         <v>61</v>
       </c>
       <c r="E140" s="9" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="F140" s="9" t="s">
         <v>11</v>
@@ -3841,7 +3929,7 @@
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>50</v>
@@ -3864,7 +3952,7 @@
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>50</v>
@@ -3876,18 +3964,18 @@
         <v>61</v>
       </c>
       <c r="E142" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F142" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G142" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>50</v>
@@ -3899,18 +3987,18 @@
         <v>61</v>
       </c>
       <c r="E143" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F143" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G143" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>50</v>
@@ -3922,18 +4010,18 @@
         <v>61</v>
       </c>
       <c r="E144" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F144" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G144" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>50</v>
@@ -3945,18 +4033,18 @@
         <v>61</v>
       </c>
       <c r="E145" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F145" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G145" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>50</v>
@@ -3968,7 +4056,7 @@
         <v>27</v>
       </c>
       <c r="E146" s="9" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="F146" s="9" t="s">
         <v>11</v>
@@ -3979,7 +4067,7 @@
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>50</v>
@@ -4002,7 +4090,7 @@
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>50</v>
@@ -4014,18 +4102,18 @@
         <v>27</v>
       </c>
       <c r="E148" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F148" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G148" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>50</v>
@@ -4037,18 +4125,18 @@
         <v>27</v>
       </c>
       <c r="E149" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F149" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G149" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>50</v>
@@ -4060,18 +4148,18 @@
         <v>27</v>
       </c>
       <c r="E150" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F150" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G150" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>50</v>
@@ -4083,18 +4171,18 @@
         <v>27</v>
       </c>
       <c r="E151" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F151" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G151" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>50</v>
@@ -4106,7 +4194,7 @@
         <v>35</v>
       </c>
       <c r="E152" s="9" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="F152" s="9" t="s">
         <v>11</v>
@@ -4117,7 +4205,7 @@
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>50</v>
@@ -4140,7 +4228,7 @@
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>50</v>
@@ -4152,18 +4240,18 @@
         <v>35</v>
       </c>
       <c r="E154" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F154" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G154" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>50</v>
@@ -4175,18 +4263,18 @@
         <v>35</v>
       </c>
       <c r="E155" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F155" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G155" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>50</v>
@@ -4198,18 +4286,18 @@
         <v>35</v>
       </c>
       <c r="E156" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F156" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G156" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B157" s="2" t="s">
         <v>50</v>
@@ -4221,18 +4309,18 @@
         <v>35</v>
       </c>
       <c r="E157" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F157" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G157" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B158" s="2" t="s">
         <v>50</v>
@@ -4244,18 +4332,18 @@
         <v>19</v>
       </c>
       <c r="E158" s="9" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="F158" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G158" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B159" s="2" t="s">
         <v>50</v>
@@ -4273,12 +4361,12 @@
         <v>11</v>
       </c>
       <c r="G159" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>50</v>
@@ -4290,24 +4378,24 @@
         <v>19</v>
       </c>
       <c r="E160" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F160" s="9" t="s">
         <v>11</v>
       </c>
       <c r="G160" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C161" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D161" s="0" t="s">
         <v>0</v>
@@ -4331,10 +4419,30 @@
       <c r="AMJ162" s="0"/>
     </row>
     <row r="163" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="10"/>
-      <c r="B163" s="11"/>
-      <c r="E163" s="13"/>
-      <c r="F163" s="13"/>
+      <c r="A163" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C163" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D163" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="E163" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F163" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G163" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="H163" s="0"/>
+      <c r="I163" s="0"/>
+      <c r="J163" s="0"/>
       <c r="AMD163" s="0"/>
       <c r="AME163" s="0"/>
       <c r="AMF163" s="0"/>
@@ -4343,156 +4451,216 @@
       <c r="AMI163" s="0"/>
       <c r="AMJ163" s="0"/>
     </row>
-    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C164" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D164" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E164" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F164" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G164" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="H164" s="0"/>
+      <c r="I164" s="0"/>
+      <c r="J164" s="0"/>
+      <c r="AMD164" s="0"/>
+      <c r="AME164" s="0"/>
+      <c r="AMF164" s="0"/>
+      <c r="AMG164" s="0"/>
+      <c r="AMH164" s="0"/>
+      <c r="AMI164" s="0"/>
+      <c r="AMJ164" s="0"/>
+    </row>
+    <row r="165" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C165" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D165" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E165" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F165" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G165" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="H165" s="0"/>
+      <c r="I165" s="0"/>
+      <c r="J165" s="0"/>
+      <c r="AMD165" s="0"/>
+      <c r="AME165" s="0"/>
+      <c r="AMF165" s="0"/>
+      <c r="AMG165" s="0"/>
+      <c r="AMH165" s="0"/>
+      <c r="AMI165" s="0"/>
+      <c r="AMJ165" s="0"/>
+    </row>
+    <row r="166" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C166" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D166" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E166" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F166" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G166" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H166" s="0"/>
+      <c r="I166" s="0"/>
+      <c r="J166" s="0"/>
+      <c r="AMD166" s="0"/>
+      <c r="AME166" s="0"/>
+      <c r="AMF166" s="0"/>
+      <c r="AMG166" s="0"/>
+      <c r="AMH166" s="0"/>
+      <c r="AMI166" s="0"/>
+      <c r="AMJ166" s="0"/>
+    </row>
+    <row r="167" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C167" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D167" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="B164" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C164" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D164" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E164" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F164" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G164" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C165" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D165" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E165" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F165" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G165" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C166" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D166" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E166" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F166" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G166" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C167" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D167" s="0" t="s">
-        <v>44</v>
-      </c>
       <c r="E167" s="9" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="F167" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G167" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G167" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="H167" s="0"/>
+      <c r="I167" s="0"/>
+      <c r="J167" s="0"/>
+      <c r="AMD167" s="0"/>
+      <c r="AME167" s="0"/>
+      <c r="AMF167" s="0"/>
+      <c r="AMG167" s="0"/>
+      <c r="AMH167" s="0"/>
+      <c r="AMI167" s="0"/>
+      <c r="AMJ167" s="0"/>
+    </row>
+    <row r="168" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D168" s="0" t="s">
-        <v>35</v>
+        <v>130</v>
       </c>
       <c r="E168" s="9" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="F168" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G168" s="0" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G168" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="H168" s="0"/>
+      <c r="I168" s="0"/>
+      <c r="J168" s="0"/>
+      <c r="AMD168" s="0"/>
+      <c r="AME168" s="0"/>
+      <c r="AMF168" s="0"/>
+      <c r="AMG168" s="0"/>
+      <c r="AMH168" s="0"/>
+      <c r="AMI168" s="0"/>
+      <c r="AMJ168" s="0"/>
+    </row>
+    <row r="169" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="C169" s="0" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D169" s="0" t="s">
-        <v>38</v>
+        <v>132</v>
       </c>
       <c r="E169" s="9" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="F169" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G169" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G169" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="H169" s="0"/>
+      <c r="I169" s="0"/>
+      <c r="J169" s="0"/>
+      <c r="AMD169" s="0"/>
+      <c r="AME169" s="0"/>
+      <c r="AMF169" s="0"/>
+      <c r="AMG169" s="0"/>
+      <c r="AMH169" s="0"/>
+      <c r="AMI169" s="0"/>
+      <c r="AMJ169" s="0"/>
+    </row>
+    <row r="170" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="C170" s="0" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="D170" s="0" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="E170" s="9" t="s">
         <v>13</v>
@@ -4501,37 +4669,57 @@
         <v>11</v>
       </c>
       <c r="G170" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C171" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D171" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E171" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F171" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G171" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="172" s="21" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="19"/>
-      <c r="B172" s="20"/>
-      <c r="E172" s="22"/>
-      <c r="F172" s="22"/>
+        <v>67</v>
+      </c>
+      <c r="H170" s="0"/>
+      <c r="I170" s="0"/>
+      <c r="J170" s="0"/>
+      <c r="AMD170" s="0"/>
+      <c r="AME170" s="0"/>
+      <c r="AMF170" s="0"/>
+      <c r="AMG170" s="0"/>
+      <c r="AMH170" s="0"/>
+      <c r="AMI170" s="0"/>
+      <c r="AMJ170" s="0"/>
+    </row>
+    <row r="171" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="10"/>
+      <c r="B171" s="11"/>
+      <c r="E171" s="13"/>
+      <c r="F171" s="13"/>
+      <c r="AMD171" s="0"/>
+      <c r="AME171" s="0"/>
+      <c r="AMF171" s="0"/>
+      <c r="AMG171" s="0"/>
+      <c r="AMH171" s="0"/>
+      <c r="AMI171" s="0"/>
+      <c r="AMJ171" s="0"/>
+    </row>
+    <row r="172" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C172" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D172" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E172" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F172" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G172" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H172" s="0"/>
+      <c r="I172" s="0"/>
+      <c r="J172" s="0"/>
       <c r="AMD172" s="0"/>
       <c r="AME172" s="0"/>
       <c r="AMF172" s="0"/>
@@ -4539,6 +4727,580 @@
       <c r="AMH172" s="0"/>
       <c r="AMI172" s="0"/>
       <c r="AMJ172" s="0"/>
+    </row>
+    <row r="173" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C173" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D173" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="E173" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F173" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G173" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="H173" s="0"/>
+      <c r="I173" s="0"/>
+      <c r="J173" s="0"/>
+      <c r="AMD173" s="0"/>
+      <c r="AME173" s="0"/>
+      <c r="AMF173" s="0"/>
+      <c r="AMG173" s="0"/>
+      <c r="AMH173" s="0"/>
+      <c r="AMI173" s="0"/>
+      <c r="AMJ173" s="0"/>
+    </row>
+    <row r="174" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C174" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D174" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E174" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F174" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G174" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="H174" s="0"/>
+      <c r="I174" s="0"/>
+      <c r="J174" s="0"/>
+      <c r="AMD174" s="0"/>
+      <c r="AME174" s="0"/>
+      <c r="AMF174" s="0"/>
+      <c r="AMG174" s="0"/>
+      <c r="AMH174" s="0"/>
+      <c r="AMI174" s="0"/>
+      <c r="AMJ174" s="0"/>
+    </row>
+    <row r="175" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C175" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D175" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E175" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F175" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G175" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="H175" s="0"/>
+      <c r="I175" s="0"/>
+      <c r="J175" s="0"/>
+      <c r="AMD175" s="0"/>
+      <c r="AME175" s="0"/>
+      <c r="AMF175" s="0"/>
+      <c r="AMG175" s="0"/>
+      <c r="AMH175" s="0"/>
+      <c r="AMI175" s="0"/>
+      <c r="AMJ175" s="0"/>
+    </row>
+    <row r="176" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C176" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D176" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E176" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F176" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G176" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="H176" s="0"/>
+      <c r="I176" s="0"/>
+      <c r="J176" s="0"/>
+      <c r="AMD176" s="0"/>
+      <c r="AME176" s="0"/>
+      <c r="AMF176" s="0"/>
+      <c r="AMG176" s="0"/>
+      <c r="AMH176" s="0"/>
+      <c r="AMI176" s="0"/>
+      <c r="AMJ176" s="0"/>
+    </row>
+    <row r="177" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C177" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D177" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E177" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F177" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G177" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="H177" s="0"/>
+      <c r="I177" s="0"/>
+      <c r="J177" s="0"/>
+      <c r="AMD177" s="0"/>
+      <c r="AME177" s="0"/>
+      <c r="AMF177" s="0"/>
+      <c r="AMG177" s="0"/>
+      <c r="AMH177" s="0"/>
+      <c r="AMI177" s="0"/>
+      <c r="AMJ177" s="0"/>
+    </row>
+    <row r="178" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C178" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D178" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E178" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F178" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G178" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H178" s="0"/>
+      <c r="I178" s="0"/>
+      <c r="J178" s="0"/>
+      <c r="AMD178" s="0"/>
+      <c r="AME178" s="0"/>
+      <c r="AMF178" s="0"/>
+      <c r="AMG178" s="0"/>
+      <c r="AMH178" s="0"/>
+      <c r="AMI178" s="0"/>
+      <c r="AMJ178" s="0"/>
+    </row>
+    <row r="179" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C179" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D179" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="E179" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F179" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G179" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="H179" s="0"/>
+      <c r="I179" s="0"/>
+      <c r="J179" s="0"/>
+      <c r="AMD179" s="0"/>
+      <c r="AME179" s="0"/>
+      <c r="AMF179" s="0"/>
+      <c r="AMG179" s="0"/>
+      <c r="AMH179" s="0"/>
+      <c r="AMI179" s="0"/>
+      <c r="AMJ179" s="0"/>
+    </row>
+    <row r="180" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C180" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D180" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E180" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F180" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G180" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H180" s="0"/>
+      <c r="I180" s="0"/>
+      <c r="J180" s="0"/>
+      <c r="AMD180" s="0"/>
+      <c r="AME180" s="0"/>
+      <c r="AMF180" s="0"/>
+      <c r="AMG180" s="0"/>
+      <c r="AMH180" s="0"/>
+      <c r="AMI180" s="0"/>
+      <c r="AMJ180" s="0"/>
+    </row>
+    <row r="181" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C181" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D181" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="E181" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F181" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G181" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="H181" s="0"/>
+      <c r="I181" s="0"/>
+      <c r="J181" s="0"/>
+      <c r="AMD181" s="0"/>
+      <c r="AME181" s="0"/>
+      <c r="AMF181" s="0"/>
+      <c r="AMG181" s="0"/>
+      <c r="AMH181" s="0"/>
+      <c r="AMI181" s="0"/>
+      <c r="AMJ181" s="0"/>
+    </row>
+    <row r="182" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C182" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D182" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E182" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F182" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G182" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="H182" s="0"/>
+      <c r="I182" s="0"/>
+      <c r="J182" s="0"/>
+      <c r="AMD182" s="0"/>
+      <c r="AME182" s="0"/>
+      <c r="AMF182" s="0"/>
+      <c r="AMG182" s="0"/>
+      <c r="AMH182" s="0"/>
+      <c r="AMI182" s="0"/>
+      <c r="AMJ182" s="0"/>
+    </row>
+    <row r="183" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C183" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D183" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E183" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F183" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G183" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="H183" s="0"/>
+      <c r="I183" s="0"/>
+      <c r="J183" s="0"/>
+      <c r="AMD183" s="0"/>
+      <c r="AME183" s="0"/>
+      <c r="AMF183" s="0"/>
+      <c r="AMG183" s="0"/>
+      <c r="AMH183" s="0"/>
+      <c r="AMI183" s="0"/>
+      <c r="AMJ183" s="0"/>
+    </row>
+    <row r="184" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="10"/>
+      <c r="B184" s="11"/>
+      <c r="E184" s="13"/>
+      <c r="F184" s="13"/>
+      <c r="J184" s="0"/>
+      <c r="AMD184" s="0"/>
+      <c r="AME184" s="0"/>
+      <c r="AMF184" s="0"/>
+      <c r="AMG184" s="0"/>
+      <c r="AMH184" s="0"/>
+      <c r="AMI184" s="0"/>
+      <c r="AMJ184" s="0"/>
+    </row>
+    <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C185" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D185" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E185" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F185" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G185" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C186" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D186" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E186" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F186" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G186" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C187" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D187" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E187" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F187" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G187" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C188" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D188" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E188" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F188" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G188" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C189" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D189" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E189" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F189" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G189" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C190" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D190" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E190" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F190" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G190" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C191" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D191" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E191" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F191" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G191" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C192" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D192" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E192" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F192" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G192" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="193" s="21" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="19"/>
+      <c r="B193" s="20"/>
+      <c r="E193" s="22"/>
+      <c r="F193" s="22"/>
+      <c r="AMD193" s="0"/>
+      <c r="AME193" s="0"/>
+      <c r="AMF193" s="0"/>
+      <c r="AMG193" s="0"/>
+      <c r="AMH193" s="0"/>
+      <c r="AMI193" s="0"/>
+      <c r="AMJ193" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4564,7 +5326,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.093023255814"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>